<commit_message>
Andi Mandi Sandi, iske agge changes karane wala
</commit_message>
<xml_diff>
--- a/ISD - EXAMPLE 1 (2).xlsx
+++ b/ISD - EXAMPLE 1 (2).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aniket\Documents\1_Python\PyCharm\1_Python-Codes\Advance-Excel-Sorter\AD-SET--Advance-Data-Sorting-Exporting-Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78A5F5BB-ED2C-4C31-8ABA-28C4BD616B4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52AA89F7-7F61-4BA6-9D5C-BB887056E902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="181" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="181" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -683,7 +683,7 @@
   <dimension ref="A1:AA7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="AA1" sqref="AA1:AA2"/>
+      <selection activeCell="V8" sqref="V8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -879,10 +879,10 @@
         <v>25</v>
       </c>
       <c r="S3">
-        <v>360.77</v>
+        <v>222</v>
       </c>
       <c r="T3">
-        <v>500</v>
+        <v>600</v>
       </c>
       <c r="V3">
         <v>25</v>
@@ -957,10 +957,10 @@
         <v>0</v>
       </c>
       <c r="S4">
-        <v>430</v>
+        <v>100</v>
       </c>
       <c r="U4">
-        <v>844</v>
+        <v>744</v>
       </c>
       <c r="V4">
         <v>0</v>
@@ -1035,10 +1035,10 @@
         <v>0</v>
       </c>
       <c r="S5">
-        <v>622</v>
+        <v>333</v>
       </c>
       <c r="T5">
-        <v>311</v>
+        <v>450</v>
       </c>
       <c r="V5">
         <v>0</v>
@@ -1116,10 +1116,10 @@
         <v>0</v>
       </c>
       <c r="T6">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="V6">
-        <v>500</v>
+        <v>700</v>
       </c>
       <c r="W6">
         <f>SUM(O6,P6,Q6,R6)</f>
@@ -1191,13 +1191,13 @@
         <v>600</v>
       </c>
       <c r="S7">
-        <v>222</v>
+        <v>560</v>
       </c>
       <c r="U7">
-        <v>366</v>
+        <v>766</v>
       </c>
       <c r="V7">
-        <v>600</v>
+        <v>987</v>
       </c>
       <c r="W7">
         <f>SUM(O7,P7,Q7,R7)</f>
@@ -1218,11 +1218,12 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="W1:W2"/>
-    <mergeCell ref="X1:X2"/>
-    <mergeCell ref="Y1:Y2"/>
-    <mergeCell ref="Z1:Z2"/>
-    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="O1:R1"/>
+    <mergeCell ref="S1:V1"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="L1:L2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
@@ -1233,12 +1234,11 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="O1:R1"/>
-    <mergeCell ref="S1:V1"/>
-    <mergeCell ref="N1:N2"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="W1:W2"/>
+    <mergeCell ref="X1:X2"/>
+    <mergeCell ref="Y1:Y2"/>
+    <mergeCell ref="Z1:Z2"/>
+    <mergeCell ref="AA1:AA2"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>

</xml_diff>